<commit_message>
+ Add language information in issues array + Transform message for directory creation from ERROR to WARN
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CNES-PLUGIN\sonar-report-cnes\src\main\resources\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835"/>
+    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
@@ -18,13 +13,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Rule</t>
   </si>
@@ -61,11 +56,14 @@
   <si>
     <t>Colonne1</t>
   </si>
+  <si>
+    <t>Language</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,11 +591,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -633,7 +631,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="42893.38993125" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="42978.618814930553" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
@@ -644,19 +642,19 @@
         <s v="python:FunctionComplexity" u="1"/>
         <s v="python:S1066" u="1"/>
         <s v="python:S134" u="1"/>
+        <s v="python:S107" u="1"/>
         <s v="python:S125" u="1"/>
-        <s v="python:S107" u="1"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Message" numFmtId="0">
+    <cacheField name="Message" numFmtId="4">
       <sharedItems containsNonDate="0" containsBlank="1" count="7">
         <m/>
-        <s v="Function &quot;generate_spaceship&quot; has 11 parameters, which is greater than the 7 authorized." u="1"/>
         <s v="Remove this commented out code." u="1"/>
-        <s v="Merge this if statement with the enclosing one." u="1"/>
-        <s v="Refactor this code to not nest more than 3 &quot;if&quot;, &quot;for&quot;, &quot;while&quot;, &quot;try&quot; and &quot;with&quot; statements." u="1"/>
         <s v="Function has a complexity of 11 which is greater than 10 authorized." u="1"/>
         <s v="Function has a complexity of 47 which is greater than 10 authorized." u="1"/>
+        <s v="Function &quot;generate_spaceship&quot; has 11 parameters, which is greater than the 7 authorized." u="1"/>
+        <s v="Refactor this code to not nest more than 3 &quot;if&quot;, &quot;for&quot;, &quot;while&quot;, &quot;try&quot; and &quot;with&quot; statements." u="1"/>
+        <s v="Merge this if statement with the enclosing one." u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
@@ -677,7 +675,7 @@
     <cacheField name="Line" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Debt" numFmtId="0">
+    <cacheField name="Effort" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -704,15 +702,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item m="1" x="1"/>
         <item m="1" x="2"/>
+        <item m="1" x="4"/>
         <item m="1" x="5"/>
-        <item m="1" x="4"/>
         <item m="1" x="3"/>
         <item x="0"/>
         <item t="default"/>
@@ -720,12 +718,12 @@
     </pivotField>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="8">
-        <item m="1" x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="6"/>
-        <item m="1" x="3"/>
         <item m="1" x="4"/>
         <item m="1" x="2"/>
+        <item m="1" x="3"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -790,13 +788,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:G2"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H2"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Rule"/>
     <tableColumn id="2" name="Message" dataDxfId="1"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Severity"/>
+    <tableColumn id="8" name="Language"/>
     <tableColumn id="5" name="File"/>
     <tableColumn id="6" name="Line"/>
     <tableColumn id="7" name="Effort"/>
@@ -858,7 +857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -891,26 +890,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -943,23 +925,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1139,7 +1104,7 @@
   <sheetPr codeName="pivotTable"/>
   <dimension ref="A3:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1195,20 +1160,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="selectedIssues"/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,19 +1188,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unconfirmed issues exported + as requested won't fix and false positive issues are exported in a new tab in XLSX file
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="1"/>
+    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
     <sheet name="All" sheetId="2" r:id="rId3"/>
+    <sheet name="Unconfirmed" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="39" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Rule</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -542,7 +546,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -562,6 +566,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -607,7 +614,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -631,11 +644,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="42978.618814930553" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="43005.394471180553" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
-  <cacheFields count="7">
+  <cacheFields count="9">
     <cacheField name="Rule" numFmtId="0">
       <sharedItems containsNonDate="0" containsBlank="1" count="6">
         <m/>
@@ -669,6 +682,11 @@
         <s v="MAJOR" u="1"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="Language" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="File" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -676,6 +694,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Effort" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Status" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -694,6 +715,8 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
+    <x v="0"/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -702,9 +725,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item m="1" x="1"/>
@@ -742,27 +765,37 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="4">
+  <rowFields count="5">
+    <field x="4"/>
     <field x="2"/>
     <field x="3"/>
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
-      <x v="1"/>
+      <x/>
     </i>
     <i r="1">
       <x v="1"/>
     </i>
     <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
       <x v="5"/>
     </i>
-    <i r="3">
+    <i r="4">
       <x v="6"/>
     </i>
     <i t="grand">
@@ -788,27 +821,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:H2"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:I2"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="1"/>
+    <tableColumn id="2" name="Message" dataDxfId="3"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Severity"/>
     <tableColumn id="8" name="Language"/>
     <tableColumn id="5" name="File"/>
     <tableColumn id="6" name="Line"/>
     <tableColumn id="7" name="Effort"/>
+    <tableColumn id="9" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:A2"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Colonne1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I2"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Rule"/>
+    <tableColumn id="2" name="Message" dataDxfId="0"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Severity"/>
+    <tableColumn id="8" name="Language"/>
+    <tableColumn id="5" name="File"/>
+    <tableColumn id="6" name="Line"/>
+    <tableColumn id="7" name="Effort"/>
+    <tableColumn id="9" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1102,10 +1154,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="pivotTable"/>
-  <dimension ref="A3:B8"/>
+  <dimension ref="A3:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,10 +1199,16 @@
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1160,10 +1218,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="selectedIssues"/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1232,7 @@
     <col min="6" max="6" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1199,11 +1257,14 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
     </row>
   </sheetData>
@@ -1245,4 +1306,64 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #9 & fix #7 + Enhance display
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\begarco\cnesreport\sonar-cnes-report\src\main\resources\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{A8D77D61-0A09-4B30-9961-DFF5D9114F6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="3"/>
+    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
@@ -14,13 +20,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="39" r:id="rId5"/>
+    <pivotCache cacheId="7" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Rule</t>
   </si>
@@ -63,11 +69,14 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>Comments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,11 +607,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -644,7 +653,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="43005.394471180553" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="43374.037758796294" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF27000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
@@ -709,7 +718,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -725,7 +734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="synthesis" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -821,46 +830,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:I2"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="3"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Severity"/>
-    <tableColumn id="8" name="Language"/>
-    <tableColumn id="5" name="File"/>
-    <tableColumn id="6" name="Line"/>
-    <tableColumn id="7" name="Effort"/>
-    <tableColumn id="9" name="Status"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rule"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Message" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Severity"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Language"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="File"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Line"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effort"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Status"/>
+    <tableColumn id="10" xr3:uid="{ECD7FBFF-2911-43D1-A7B1-9BD75AE9511A}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Colonne1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:I2"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="0"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Severity"/>
-    <tableColumn id="8" name="Language"/>
-    <tableColumn id="5" name="File"/>
-    <tableColumn id="6" name="Line"/>
-    <tableColumn id="7" name="Effort"/>
-    <tableColumn id="9" name="Status"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Rule"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Severity"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Language"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="File"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Line"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Effort"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Status"/>
+    <tableColumn id="10" xr3:uid="{2C6AAEB9-4103-4F44-A14E-E358A5B26A34}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -909,7 +920,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -942,9 +953,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,6 +1005,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1152,12 +1197,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="pivotTable"/>
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,12 +1261,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="selectedIssues"/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,9 +1275,10 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1260,11 +1306,14 @@
       <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
     </row>
   </sheetData>
@@ -1276,7 +1325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="allIssues"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1309,11 +1358,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,9 +1371,10 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1352,16 +1402,19 @@
       <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Add hotspot support for 8.X+ to xlsx fix #133
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labo\IdeaProjects\sonar-cnes-report\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amthomas/dev/testing/en-report/sonar-cnes-report/src/main/resources/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5837C2-E85B-4E48-A3C9-8DD61C0DCCF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="4"/>
+    <workbookView xWindow="760" yWindow="520" windowWidth="19880" windowHeight="12560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
     <sheet name="All" sheetId="2" r:id="rId3"/>
     <sheet name="Unconfirmed" sheetId="4" r:id="rId4"/>
-    <sheet name="Metrics" sheetId="5" r:id="rId5"/>
+    <sheet name="Hotspots" sheetId="6" r:id="rId5"/>
+    <sheet name="Metrics" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="79" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Rule</t>
   </si>
@@ -46,16 +48,7 @@
     <t>Line</t>
   </si>
   <si>
-    <t>Étiquettes de lignes</t>
-  </si>
-  <si>
-    <t>Total général</t>
-  </si>
-  <si>
     <t>Nombre de Message</t>
-  </si>
-  <si>
-    <t>(vide)</t>
   </si>
   <si>
     <t>Effort</t>
@@ -72,11 +65,20 @@
   <si>
     <t>Comments</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,50 +582,53 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -656,7 +661,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="labo" refreshedDate="43571.447895833335" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Aaron Thomas" refreshedDate="43972.002707754633" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF07000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
@@ -724,7 +729,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -741,7 +746,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="synthesis" cacheId="79" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -838,65 +843,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:J2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="4"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Severity"/>
-    <tableColumn id="8" name="Language"/>
-    <tableColumn id="5" name="File"/>
-    <tableColumn id="6" name="Line"/>
-    <tableColumn id="7" name="Effort"/>
-    <tableColumn id="9" name="Status"/>
-    <tableColumn id="10" name="Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rule"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Message" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Severity"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Language"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="File"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Line"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effort"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Status"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Colonne1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:J2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="1"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Severity"/>
-    <tableColumn id="8" name="Language"/>
-    <tableColumn id="5" name="File"/>
-    <tableColumn id="6" name="Line"/>
-    <tableColumn id="7" name="Effort"/>
-    <tableColumn id="9" name="Status"/>
-    <tableColumn id="10" name="Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Rule"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Severity"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Language"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="File"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Line"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Effort"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Status"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="metrics" displayName="metrics" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7C0E2B34-BAF6-6345-88D7-2F6A226ECE53}" name="hotspots" displayName="hotspots" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Colonne1"/>
+    <tableColumn id="1" xr3:uid="{13BEF51C-EF80-264A-8DDE-E3150A0A8CC2}" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="metrics" displayName="metrics" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Colonne1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -971,6 +986,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1006,6 +1038,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1181,7 +1230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="pivotTable"/>
   <dimension ref="A3:B9"/>
   <sheetViews>
@@ -1189,53 +1238,53 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B9" s="7"/>
     </row>
@@ -1245,7 +1294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="selectedIssues"/>
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1253,16 +1302,16 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1285,19 +1334,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
     </row>
   </sheetData>
@@ -1309,7 +1358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="allIssues"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1317,19 +1366,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1342,23 +1391,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1421,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1381,19 +1430,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
     </row>
   </sheetData>
@@ -1406,24 +1455,56 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A53885-0649-3F4C-8935-9B0FEA133949}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue #134 on xlsx template
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labo\IdeaProjects\sonar-cnes-report\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labo\sonar-cnes-report\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="4"/>
+    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
@@ -656,7 +656,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="labo" refreshedDate="43571.447895833335" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="labo" refreshedDate="44004.650755787035" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
@@ -1185,7 +1185,7 @@
   <sheetPr codeName="pivotTable"/>
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1409,7 +1409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
add security hotspots to excel report
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labo\sonar-cnes-report\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauduce\Desktop\New Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,17 +16,18 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
     <sheet name="All" sheetId="2" r:id="rId3"/>
     <sheet name="Unconfirmed" sheetId="4" r:id="rId4"/>
-    <sheet name="Metrics" sheetId="5" r:id="rId5"/>
+    <sheet name="Security Hotspots" sheetId="6" r:id="rId5"/>
+    <sheet name="Metrics" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>Rule</t>
   </si>
@@ -71,6 +72,15 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Resolution</t>
   </si>
 </sst>
 </file>
@@ -623,7 +633,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -656,7 +672,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="labo" refreshedDate="44004.650755787035" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Gauduchon Erwan" refreshedDate="44313.646445833336" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
@@ -838,11 +854,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:J2"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="4"/>
+    <tableColumn id="2" name="Message" dataDxfId="6"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Severity"/>
     <tableColumn id="8" name="Language"/>
@@ -857,7 +873,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:A2"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Colonne1"/>
@@ -867,11 +883,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:J2"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Rule"/>
-    <tableColumn id="2" name="Message" dataDxfId="1"/>
+    <tableColumn id="2" name="Message" dataDxfId="3"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Severity"/>
     <tableColumn id="8" name="Language"/>
@@ -886,6 +902,26 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="hotspots" displayName="hotspots" ref="A1:K2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:K2"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Rule"/>
+    <tableColumn id="2" name="Message" dataDxfId="1"/>
+    <tableColumn id="3" name="Category"/>
+    <tableColumn id="12" name="Priority"/>
+    <tableColumn id="4" name="Severity"/>
+    <tableColumn id="8" name="Language"/>
+    <tableColumn id="5" name="File"/>
+    <tableColumn id="6" name="Line"/>
+    <tableColumn id="9" name="Status"/>
+    <tableColumn id="13" name="Resolution"/>
+    <tableColumn id="10" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="metrics" displayName="metrics" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:A2"/>
   <tableColumns count="1">
@@ -1407,6 +1443,70 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>